<commit_message>
poc 1 training 2
</commit_message>
<xml_diff>
--- a/Input_Data/validation_rbi.xlsx
+++ b/Input_Data/validation_rbi.xlsx
@@ -2623,17 +2623,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="16" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="16" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="16" width="41.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="16" width="35.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="16" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="16" width="24.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="16" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="16" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="16" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="16" width="38.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="16" width="40.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="16" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="16" width="10.005" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="16" width="110.7192857142857" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="16" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="16" width="13.005" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="16" width="55.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="16" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="16" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="16" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="16" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -3039,7 +3039,7 @@
       </c>
       <c r="K13" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="5" t="s">
         <v>83</v>
       </c>
@@ -3070,7 +3070,7 @@
       </c>
       <c r="K14" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="5" t="s">
         <v>86</v>
       </c>
@@ -3099,7 +3099,7 @@
       </c>
       <c r="K15" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="5" t="s">
         <v>91</v>
       </c>
@@ -3130,7 +3130,7 @@
       </c>
       <c r="K16" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="5" t="s">
         <v>96</v>
       </c>
@@ -3159,7 +3159,7 @@
       </c>
       <c r="K17" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="30">
       <c r="A18" s="5" t="s">
         <v>102</v>
       </c>
@@ -3192,7 +3192,7 @@
       </c>
       <c r="K18" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="5" t="s">
         <v>108</v>
       </c>
@@ -3223,7 +3223,7 @@
       </c>
       <c r="K19" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="5" t="s">
         <v>113</v>
       </c>
@@ -3254,7 +3254,7 @@
       </c>
       <c r="K20" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="5" t="s">
         <v>113</v>
       </c>
@@ -3285,7 +3285,7 @@
       </c>
       <c r="K21" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="5" t="s">
         <v>121</v>
       </c>
@@ -3314,7 +3314,7 @@
       </c>
       <c r="K22" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="5" t="s">
         <v>127</v>
       </c>
@@ -3345,7 +3345,7 @@
       </c>
       <c r="K23" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="5" t="s">
         <v>132</v>
       </c>
@@ -3376,7 +3376,7 @@
       </c>
       <c r="K24" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5">
       <c r="A25" s="5" t="s">
         <v>137</v>
       </c>
@@ -3407,7 +3407,7 @@
       </c>
       <c r="K25" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18">
       <c r="A26" s="5" t="s">
         <v>144</v>
       </c>
@@ -3438,7 +3438,7 @@
       </c>
       <c r="K26" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18">
       <c r="A27" s="5" t="s">
         <v>150</v>
       </c>
@@ -3469,7 +3469,7 @@
       </c>
       <c r="K27" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18">
       <c r="A28" s="5" t="s">
         <v>154</v>
       </c>
@@ -3498,7 +3498,7 @@
       </c>
       <c r="K28" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18">
       <c r="A29" s="5" t="s">
         <v>158</v>
       </c>
@@ -3529,7 +3529,7 @@
       </c>
       <c r="K29" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18">
       <c r="A30" s="5" t="s">
         <v>164</v>
       </c>
@@ -3560,7 +3560,7 @@
       </c>
       <c r="K30" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18">
       <c r="A31" s="5" t="s">
         <v>171</v>
       </c>
@@ -3593,7 +3593,7 @@
       </c>
       <c r="K31" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18">
       <c r="A32" s="5" t="s">
         <v>176</v>
       </c>
@@ -3626,7 +3626,7 @@
       </c>
       <c r="K32" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18">
       <c r="A33" s="5" t="s">
         <v>182</v>
       </c>
@@ -3657,7 +3657,7 @@
       </c>
       <c r="K33" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18">
       <c r="A34" s="5" t="s">
         <v>189</v>
       </c>
@@ -3688,7 +3688,7 @@
       </c>
       <c r="K34" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18">
       <c r="A35" s="5" t="s">
         <v>194</v>
       </c>
@@ -3717,7 +3717,7 @@
       </c>
       <c r="K35" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18">
       <c r="A36" s="5" t="s">
         <v>199</v>
       </c>
@@ -3748,7 +3748,7 @@
       </c>
       <c r="K36" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18">
       <c r="A37" s="5" t="s">
         <v>204</v>
       </c>
@@ -3779,7 +3779,7 @@
       </c>
       <c r="K37" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18">
       <c r="A38" s="5" t="s">
         <v>209</v>
       </c>
@@ -3810,7 +3810,7 @@
       </c>
       <c r="K38" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18">
       <c r="A39" s="5" t="s">
         <v>214</v>
       </c>
@@ -3839,7 +3839,7 @@
       </c>
       <c r="K39" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18">
       <c r="A40" s="5" t="s">
         <v>218</v>
       </c>
@@ -3868,7 +3868,7 @@
       </c>
       <c r="K40" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18">
       <c r="A41" s="5" t="s">
         <v>222</v>
       </c>
@@ -3897,7 +3897,7 @@
       </c>
       <c r="K41" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18">
       <c r="A42" s="5" t="s">
         <v>226</v>
       </c>
@@ -3926,7 +3926,7 @@
       </c>
       <c r="K42" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18">
       <c r="A43" s="5" t="s">
         <v>230</v>
       </c>
@@ -3957,7 +3957,7 @@
       </c>
       <c r="K43" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18">
       <c r="A44" s="5" t="s">
         <v>237</v>
       </c>
@@ -3988,7 +3988,7 @@
       </c>
       <c r="K44" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18">
       <c r="A45" s="5" t="s">
         <v>242</v>
       </c>
@@ -4019,7 +4019,7 @@
       </c>
       <c r="K45" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18">
       <c r="A46" s="5" t="s">
         <v>248</v>
       </c>
@@ -4050,7 +4050,7 @@
       </c>
       <c r="K46" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18">
       <c r="A47" s="5" t="s">
         <v>253</v>
       </c>
@@ -4081,7 +4081,7 @@
       </c>
       <c r="K47" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18">
       <c r="A48" s="5" t="s">
         <v>259</v>
       </c>
@@ -4112,7 +4112,7 @@
       </c>
       <c r="K48" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18">
       <c r="A49" s="5" t="s">
         <v>264</v>
       </c>
@@ -4145,7 +4145,7 @@
       </c>
       <c r="K49" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18">
       <c r="A50" s="5" t="s">
         <v>269</v>
       </c>
@@ -4178,7 +4178,7 @@
       </c>
       <c r="K50" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18">
       <c r="A51" s="5" t="s">
         <v>276</v>
       </c>
@@ -4211,7 +4211,7 @@
       </c>
       <c r="K51" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18">
       <c r="A52" s="5" t="s">
         <v>242</v>
       </c>
@@ -4242,7 +4242,7 @@
       </c>
       <c r="K52" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18">
       <c r="A53" s="5" t="s">
         <v>285</v>
       </c>
@@ -4271,7 +4271,7 @@
       </c>
       <c r="K53" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18">
       <c r="A54" s="5" t="s">
         <v>290</v>
       </c>
@@ -4300,7 +4300,7 @@
       </c>
       <c r="K54" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18">
       <c r="A55" s="5" t="s">
         <v>296</v>
       </c>
@@ -4331,7 +4331,7 @@
       </c>
       <c r="K55" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18">
       <c r="A56" s="5" t="s">
         <v>302</v>
       </c>
@@ -4362,7 +4362,7 @@
       </c>
       <c r="K56" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18">
       <c r="A57" s="5" t="s">
         <v>308</v>
       </c>
@@ -4391,7 +4391,7 @@
       </c>
       <c r="K57" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18">
       <c r="A58" s="5" t="s">
         <v>313</v>
       </c>
@@ -4420,7 +4420,7 @@
       </c>
       <c r="K58" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18">
       <c r="A59" s="5" t="s">
         <v>319</v>
       </c>
@@ -4449,7 +4449,7 @@
       </c>
       <c r="K59" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18">
       <c r="A60" s="5" t="s">
         <v>324</v>
       </c>
@@ -4478,7 +4478,7 @@
       </c>
       <c r="K60" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18">
       <c r="A61" s="5" t="s">
         <v>328</v>
       </c>
@@ -4509,7 +4509,7 @@
       </c>
       <c r="K61" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18">
       <c r="A62" s="5" t="s">
         <v>333</v>
       </c>
@@ -4540,7 +4540,7 @@
       </c>
       <c r="K62" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18">
       <c r="A63" s="5" t="s">
         <v>91</v>
       </c>
@@ -4573,7 +4573,7 @@
       </c>
       <c r="K63" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18">
       <c r="A64" s="5" t="s">
         <v>342</v>
       </c>
@@ -4606,7 +4606,7 @@
       </c>
       <c r="K64" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18">
       <c r="A65" s="5" t="s">
         <v>348</v>
       </c>
@@ -4635,7 +4635,7 @@
       </c>
       <c r="K65" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18">
       <c r="A66" s="5" t="s">
         <v>44</v>
       </c>
@@ -4666,7 +4666,7 @@
       </c>
       <c r="K66" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18">
       <c r="A67" s="5" t="s">
         <v>355</v>
       </c>
@@ -4697,7 +4697,7 @@
       </c>
       <c r="K67" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18">
       <c r="A68" s="5" t="s">
         <v>362</v>
       </c>
@@ -4728,7 +4728,7 @@
       </c>
       <c r="K68" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18">
       <c r="A69" s="5" t="s">
         <v>368</v>
       </c>
@@ -4759,7 +4759,7 @@
       </c>
       <c r="K69" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18">
       <c r="A70" s="5" t="s">
         <v>374</v>
       </c>
@@ -4790,7 +4790,7 @@
       </c>
       <c r="K70" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18">
       <c r="A71" s="5" t="s">
         <v>379</v>
       </c>
@@ -4823,7 +4823,7 @@
       </c>
       <c r="K71" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18">
       <c r="A72" s="5" t="s">
         <v>384</v>
       </c>
@@ -4854,7 +4854,7 @@
       </c>
       <c r="K72" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18">
       <c r="A73" s="5" t="s">
         <v>390</v>
       </c>
@@ -4885,7 +4885,7 @@
       </c>
       <c r="K73" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18">
       <c r="A74" s="5" t="s">
         <v>395</v>
       </c>
@@ -4916,7 +4916,7 @@
       </c>
       <c r="K74" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18">
       <c r="A75" s="5" t="s">
         <v>400</v>
       </c>
@@ -4945,7 +4945,7 @@
       </c>
       <c r="K75" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18">
       <c r="A76" s="5" t="s">
         <v>404</v>
       </c>
@@ -4976,7 +4976,7 @@
       </c>
       <c r="K76" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18">
       <c r="A77" s="5" t="s">
         <v>408</v>
       </c>
@@ -5009,7 +5009,7 @@
       </c>
       <c r="K77" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18">
       <c r="A78" s="5" t="s">
         <v>413</v>
       </c>
@@ -5040,7 +5040,7 @@
       </c>
       <c r="K78" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18">
       <c r="A79" s="5" t="s">
         <v>418</v>
       </c>
@@ -5069,7 +5069,7 @@
       </c>
       <c r="K79" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18">
       <c r="A80" s="5" t="s">
         <v>422</v>
       </c>
@@ -5100,7 +5100,7 @@
       </c>
       <c r="K80" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18">
       <c r="A81" s="5" t="s">
         <v>427</v>
       </c>
@@ -5131,7 +5131,7 @@
       </c>
       <c r="K81" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18">
       <c r="A82" s="5" t="s">
         <v>434</v>
       </c>
@@ -5162,7 +5162,7 @@
       </c>
       <c r="K82" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18">
       <c r="A83" s="5" t="s">
         <v>441</v>
       </c>
@@ -5193,7 +5193,7 @@
       </c>
       <c r="K83" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18">
       <c r="A84" s="5" t="s">
         <v>121</v>
       </c>
@@ -5224,7 +5224,7 @@
       </c>
       <c r="K84" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18">
       <c r="A85" s="5" t="s">
         <v>450</v>
       </c>
@@ -5255,7 +5255,7 @@
       </c>
       <c r="K85" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18">
       <c r="A86" s="5" t="s">
         <v>456</v>
       </c>
@@ -5286,7 +5286,7 @@
       </c>
       <c r="K86" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18">
       <c r="A87" s="5" t="s">
         <v>463</v>
       </c>
@@ -5317,7 +5317,7 @@
       </c>
       <c r="K87" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18">
       <c r="A88" s="5" t="s">
         <v>469</v>
       </c>
@@ -5348,7 +5348,7 @@
       </c>
       <c r="K88" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18">
       <c r="A89" s="5" t="s">
         <v>474</v>
       </c>
@@ -5379,7 +5379,7 @@
       </c>
       <c r="K89" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18">
       <c r="A90" s="5" t="s">
         <v>481</v>
       </c>
@@ -5410,7 +5410,7 @@
       </c>
       <c r="K90" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18">
       <c r="A91" s="5" t="s">
         <v>486</v>
       </c>
@@ -5439,7 +5439,7 @@
       </c>
       <c r="K91" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18">
       <c r="A92" s="5" t="s">
         <v>491</v>
       </c>
@@ -5470,7 +5470,7 @@
       </c>
       <c r="K92" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18">
       <c r="A93" s="5" t="s">
         <v>498</v>
       </c>
@@ -5501,7 +5501,7 @@
       </c>
       <c r="K93" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18">
       <c r="A94" s="5" t="s">
         <v>503</v>
       </c>
@@ -5532,7 +5532,7 @@
       </c>
       <c r="K94" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18">
       <c r="A95" s="5" t="s">
         <v>509</v>
       </c>
@@ -5563,7 +5563,7 @@
       </c>
       <c r="K95" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18">
       <c r="A96" s="5" t="s">
         <v>514</v>
       </c>
@@ -5594,7 +5594,7 @@
       </c>
       <c r="K96" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18">
       <c r="A97" s="5" t="s">
         <v>519</v>
       </c>
@@ -5623,7 +5623,7 @@
       </c>
       <c r="K97" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18">
       <c r="A98" s="5" t="s">
         <v>525</v>
       </c>
@@ -5652,7 +5652,7 @@
       </c>
       <c r="K98" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18">
       <c r="A99" s="5" t="s">
         <v>529</v>
       </c>
@@ -5683,7 +5683,7 @@
       </c>
       <c r="K99" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18">
       <c r="A100" s="5" t="s">
         <v>525</v>
       </c>
@@ -5716,7 +5716,7 @@
       </c>
       <c r="K100" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18">
       <c r="A101" s="5" t="s">
         <v>539</v>
       </c>
@@ -5749,7 +5749,7 @@
       </c>
       <c r="K101" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18">
       <c r="A102" s="5" t="s">
         <v>544</v>
       </c>
@@ -5780,7 +5780,7 @@
       </c>
       <c r="K102" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18">
       <c r="A103" s="5" t="s">
         <v>551</v>
       </c>
@@ -5811,7 +5811,7 @@
       </c>
       <c r="K103" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18">
       <c r="A104" s="5" t="s">
         <v>557</v>
       </c>
@@ -5844,7 +5844,7 @@
       </c>
       <c r="K104" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18">
       <c r="A105" s="5" t="s">
         <v>49</v>
       </c>
@@ -5877,7 +5877,7 @@
       </c>
       <c r="K105" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18">
       <c r="A106" s="5" t="s">
         <v>566</v>
       </c>
@@ -5908,7 +5908,7 @@
       </c>
       <c r="K106" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18">
       <c r="A107" s="5" t="s">
         <v>572</v>
       </c>
@@ -5939,7 +5939,7 @@
       </c>
       <c r="K107" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18">
       <c r="A108" s="5" t="s">
         <v>578</v>
       </c>
@@ -5970,7 +5970,7 @@
       </c>
       <c r="K108" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18">
       <c r="A109" s="5" t="s">
         <v>584</v>
       </c>
@@ -6001,7 +6001,7 @@
       </c>
       <c r="K109" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18">
       <c r="A110" s="5" t="s">
         <v>589</v>
       </c>
@@ -6032,7 +6032,7 @@
       </c>
       <c r="K110" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18">
       <c r="A111" s="5" t="s">
         <v>594</v>
       </c>
@@ -6063,7 +6063,7 @@
       </c>
       <c r="K111" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18">
       <c r="A112" s="5" t="s">
         <v>599</v>
       </c>
@@ -6092,7 +6092,7 @@
       </c>
       <c r="K112" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18">
       <c r="A113" s="5" t="s">
         <v>603</v>
       </c>
@@ -6125,7 +6125,7 @@
       </c>
       <c r="K113" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18">
       <c r="A114" s="5" t="s">
         <v>608</v>
       </c>
@@ -6154,7 +6154,7 @@
       </c>
       <c r="K114" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18">
       <c r="A115" s="5" t="s">
         <v>613</v>
       </c>
@@ -6183,7 +6183,7 @@
       </c>
       <c r="K115" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18">
       <c r="A116" s="5" t="s">
         <v>619</v>
       </c>
@@ -6214,7 +6214,7 @@
       </c>
       <c r="K116" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18">
       <c r="A117" s="5" t="s">
         <v>599</v>
       </c>
@@ -6245,7 +6245,7 @@
       </c>
       <c r="K117" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18">
       <c r="A118" s="5" t="s">
         <v>628</v>
       </c>
@@ -6276,7 +6276,7 @@
       </c>
       <c r="K118" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18">
       <c r="A119" s="5" t="s">
         <v>634</v>
       </c>
@@ -6307,7 +6307,7 @@
       </c>
       <c r="K119" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18">
       <c r="A120" s="5" t="s">
         <v>639</v>
       </c>
@@ -6338,7 +6338,7 @@
       </c>
       <c r="K120" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18">
       <c r="A121" s="5" t="s">
         <v>645</v>
       </c>
@@ -6369,7 +6369,7 @@
       </c>
       <c r="K121" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18">
       <c r="A122" s="5" t="s">
         <v>651</v>
       </c>
@@ -6398,7 +6398,7 @@
       </c>
       <c r="K122" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18">
       <c r="A123" s="5" t="s">
         <v>656</v>
       </c>
@@ -6429,7 +6429,7 @@
       </c>
       <c r="K123" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18">
       <c r="A124" s="5" t="s">
         <v>663</v>
       </c>
@@ -6458,7 +6458,7 @@
       </c>
       <c r="K124" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18">
       <c r="A125" s="5" t="s">
         <v>668</v>
       </c>
@@ -6489,7 +6489,7 @@
       </c>
       <c r="K125" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18">
       <c r="A126" s="5" t="s">
         <v>253</v>
       </c>
@@ -6520,7 +6520,7 @@
       </c>
       <c r="K126" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18">
       <c r="A127" s="5" t="s">
         <v>677</v>
       </c>
@@ -6553,7 +6553,7 @@
       </c>
       <c r="K127" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18">
       <c r="A128" s="5" t="s">
         <v>683</v>
       </c>
@@ -6586,7 +6586,7 @@
       </c>
       <c r="K128" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18">
       <c r="A129" s="5" t="s">
         <v>688</v>
       </c>
@@ -6617,7 +6617,7 @@
       </c>
       <c r="K129" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="18">
       <c r="A130" s="5" t="s">
         <v>693</v>
       </c>
@@ -6648,7 +6648,7 @@
       </c>
       <c r="K130" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18">
       <c r="A131" s="5" t="s">
         <v>594</v>
       </c>

</xml_diff>